<commit_message>
ultimo commit antes do primeiro empacotamento
</commit_message>
<xml_diff>
--- a/modelo.xlsx
+++ b/modelo.xlsx
@@ -136,7 +136,7 @@
     <numFmt numFmtId="165" formatCode="[$-416]d/m/yyyy"/>
     <numFmt numFmtId="166" formatCode="&quot;R$ &quot;#,##0.00;[RED]&quot;-R$ &quot;#,##0.00"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -204,12 +204,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -495,7 +489,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -626,9 +620,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>567720</xdr:colOff>
+      <xdr:colOff>567360</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -642,7 +636,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="360" y="163080"/>
-          <a:ext cx="1818360" cy="653040"/>
+          <a:ext cx="1818000" cy="652680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -772,10 +766,14 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N16" activeCellId="0" sqref="N16"/>
+      <selection pane="topLeft" activeCell="P23" activeCellId="0" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="5.84"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>

</xml_diff>